<commit_message>
V0.2 Alpha Version: Add formulas to output Excel
</commit_message>
<xml_diff>
--- a/templates/template.xlsx
+++ b/templates/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal Projects\Conciliaciones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal Projects\Conciliaciones\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB10FF6-04CE-4310-85D3-FDE158F23DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE2AFE5-B0D4-4EB8-B900-3A17044FCB1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{549DB920-7ECE-407E-8B8D-07B41B1687AC}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="BBVA 0829" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'BBVA 0829'!$D$3:$H$62</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'BBVA 0829'!$D$3:$H$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,9 +67,6 @@
     <t>ABONOS DEL BANCO NO CORRESPONIDOS POR NOSOTROS</t>
   </si>
   <si>
-    <t>SALDO SEGÚN CONTABILIDAD AL 28/02/2021</t>
-  </si>
-  <si>
     <t>DIFERENCIA</t>
   </si>
   <si>
@@ -83,6 +80,9 @@
   </si>
   <si>
     <t>ESTE SE TOMA DEL ESTADO DE CTA</t>
+  </si>
+  <si>
+    <t>SALDO SEGÚN CONTABILIDAD AL dd/MM/yyyy</t>
   </si>
 </sst>
 </file>
@@ -309,46 +309,48 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -858,390 +860,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1228725</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Conector recto 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{708E2028-EAE5-4ECE-8665-A7CF007C5545}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="914400" y="9763125"/>
-          <a:ext cx="2009775" cy="19050"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2114550</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="10" name="Conector recto 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCB631D5-6BAF-4B99-8D6E-F68177AC43F1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3810000" y="9791700"/>
-          <a:ext cx="2009775" cy="19050"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1895475</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="CuadroTexto 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C158C7C6-DA47-458A-B17D-7E079217C524}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3590925" y="9839325"/>
-          <a:ext cx="2266950" cy="866775"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100" b="1">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Autorizó</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Herminio Núñez</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100" baseline="0">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> Mora</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-MX" sz="1100">
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Gerente de contabilidad</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Num de Cédula:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100" baseline="0">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> 4471823</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-MX" sz="1100">
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="es-MX" sz="1100">
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>847724</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Imagen 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C86CF9A-E759-4487-947C-1796A8032147}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:srcRect l="879" t="23101" r="43331" b="13169"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="266700" y="4533900"/>
-          <a:ext cx="6648449" cy="4467225"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1252537</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="CuadroTexto 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C80D5E93-7CB8-4613-AF48-32B232027013}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="657225" y="9848850"/>
-          <a:ext cx="2290762" cy="714375"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100" b="1">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Realizó</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Jessica Natalia Matías Martínez</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-MX" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Contadora Jr.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="es-MX" sz="1100">
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="es-MX" sz="1100">
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1546,10 +1164,10 @@
     <tabColor rgb="FF00B0F0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="D2:K62"/>
+  <dimension ref="D2:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1943,13 +1561,13 @@
   <sheetData>
     <row r="2" spans="4:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="4:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="30"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D4" s="2"/>
@@ -1959,29 +1577,29 @@
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="4:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="32"/>
+    </row>
+    <row r="6" spans="4:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="33"/>
-    </row>
-    <row r="6" spans="4:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D6" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="33"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="32"/>
     </row>
     <row r="7" spans="4:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="33"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="32"/>
     </row>
     <row r="8" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D8" s="2"/>
@@ -1997,9 +1615,11 @@
         <v>1</v>
       </c>
       <c r="G9" s="10"/>
-      <c r="H9" s="11"/>
+      <c r="H9" s="11">
+        <v>0</v>
+      </c>
       <c r="I9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="4:9" x14ac:dyDescent="0.2">
@@ -2046,7 +1666,7 @@
     </row>
     <row r="14" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D14" s="2"/>
-      <c r="E14" s="8"/>
+      <c r="E14" s="25"/>
       <c r="F14" s="6"/>
       <c r="G14" s="10"/>
       <c r="H14" s="12"/>
@@ -2067,7 +1687,7 @@
     <row r="16" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D16" s="2"/>
       <c r="E16" s="14"/>
-      <c r="F16" s="27"/>
+      <c r="F16" s="20"/>
       <c r="G16" s="10"/>
       <c r="H16" s="16"/>
       <c r="I16" s="15"/>
@@ -2088,7 +1708,7 @@
     <row r="18" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D18" s="2"/>
       <c r="E18" s="14"/>
-      <c r="F18" s="27"/>
+      <c r="F18" s="20"/>
       <c r="G18" s="10"/>
       <c r="H18" s="12"/>
     </row>
@@ -2102,210 +1722,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D20" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
+    <row r="20" spans="4:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D20" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
       <c r="H20" s="11">
-        <v>3865712.29</v>
+        <v>0</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J20" s="17"/>
       <c r="K20" s="17"/>
     </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D21" s="2"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="10"/>
-      <c r="H21" s="20">
+    <row r="21" spans="4:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D21" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="18">
         <f>H19-H20</f>
-        <v>-3865712.29</v>
-      </c>
-      <c r="J21" s="21"/>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D22" s="2"/>
-      <c r="H22" s="22"/>
-      <c r="J22" s="17"/>
-    </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D23" s="2"/>
-      <c r="H23" s="23"/>
-    </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D24" s="2"/>
-      <c r="H24" s="22"/>
-    </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D25" s="2"/>
-      <c r="H25" s="22"/>
-    </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D26" s="2"/>
-      <c r="H26" s="22"/>
-    </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D27" s="2"/>
-      <c r="H27" s="22"/>
-    </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D28" s="2"/>
-      <c r="H28" s="22"/>
-    </row>
-    <row r="29" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D29" s="2"/>
-      <c r="H29" s="22"/>
-    </row>
-    <row r="30" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D30" s="2"/>
-      <c r="H30" s="22"/>
-    </row>
-    <row r="31" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D31" s="2"/>
-      <c r="H31" s="22"/>
-    </row>
-    <row r="32" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D32" s="2"/>
-      <c r="H32" s="22"/>
-    </row>
-    <row r="33" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D33" s="2"/>
-      <c r="H33" s="22"/>
-    </row>
-    <row r="34" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D34" s="2"/>
-      <c r="H34" s="22"/>
-    </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D35" s="2"/>
-      <c r="H35" s="22"/>
-    </row>
-    <row r="36" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D36" s="2"/>
-      <c r="H36" s="22"/>
-    </row>
-    <row r="37" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D37" s="2"/>
-      <c r="H37" s="22"/>
-    </row>
-    <row r="38" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D38" s="2"/>
-      <c r="H38" s="22"/>
-    </row>
-    <row r="39" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D39" s="2"/>
-      <c r="H39" s="22"/>
-    </row>
-    <row r="40" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D40" s="2"/>
-      <c r="H40" s="22"/>
-    </row>
-    <row r="41" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D41" s="2"/>
-      <c r="H41" s="22"/>
-    </row>
-    <row r="42" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D42" s="2"/>
-      <c r="H42" s="22"/>
-    </row>
-    <row r="43" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D43" s="2"/>
-      <c r="H43" s="22"/>
-    </row>
-    <row r="44" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D44" s="2"/>
-      <c r="H44" s="22"/>
-    </row>
-    <row r="45" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D45" s="2"/>
-      <c r="H45" s="22"/>
-    </row>
-    <row r="46" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D46" s="2"/>
-      <c r="H46" s="22"/>
-    </row>
-    <row r="47" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D47" s="2"/>
-      <c r="H47" s="22"/>
-    </row>
-    <row r="48" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D48" s="2"/>
-      <c r="H48" s="22"/>
-    </row>
-    <row r="49" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D49" s="2"/>
-      <c r="H49" s="22"/>
-    </row>
-    <row r="50" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D50" s="2"/>
-      <c r="H50" s="22"/>
-    </row>
-    <row r="51" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D51" s="2"/>
-      <c r="H51" s="22"/>
-    </row>
-    <row r="52" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D52" s="2"/>
-      <c r="H52" s="22"/>
-    </row>
-    <row r="53" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D53" s="2"/>
-      <c r="H53" s="22"/>
-    </row>
-    <row r="54" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D54" s="2"/>
-      <c r="H54" s="22"/>
-    </row>
-    <row r="55" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D55" s="2"/>
-      <c r="H55" s="22"/>
-    </row>
-    <row r="56" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D56" s="2"/>
-      <c r="H56" s="22"/>
-    </row>
-    <row r="57" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D57" s="2"/>
-      <c r="H57" s="22"/>
-    </row>
-    <row r="58" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D58" s="2"/>
-      <c r="H58" s="22"/>
-    </row>
-    <row r="59" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D59" s="2"/>
-      <c r="H59" s="22"/>
-    </row>
-    <row r="60" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D60" s="2"/>
-      <c r="H60" s="22"/>
-    </row>
-    <row r="61" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D61" s="2"/>
-      <c r="H61" s="22"/>
-    </row>
-    <row r="62" spans="4:8" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D62" s="24"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="25"/>
-      <c r="G62" s="25"/>
-      <c r="H62" s="26"/>
-    </row>
+        <v>0</v>
+      </c>
+      <c r="J21" s="19"/>
+    </row>
+    <row r="22" spans="4:11" s="26" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="33"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="35"/>
+    </row>
+    <row r="23" spans="4:11" s="26" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="D3:H3"/>
     <mergeCell ref="D5:H5"/>
     <mergeCell ref="D6:H6"/>
     <mergeCell ref="D7:H7"/>
-    <mergeCell ref="D20:G20"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="86" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>